<commit_message>
Changed to Greek data
lorep ipsum just did a change
</commit_message>
<xml_diff>
--- a/Data As Is/GRC/GRC_Unicom_meds_v4.xlsx
+++ b/Data As Is/GRC/GRC_Unicom_meds_v4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haralamposkaranikas/Dropbox/0_CurrentProjects/7_Gnom_Berler/2_UNICOM/2022_11_3_Greek_Pilot_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArgirisGKOGKIDIS\Documents\GitHub\source-data\Data As Is\GRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CB6C97-2DCF-1A40-B11E-A2CE5C350583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56399620-FB64-4BE5-BFFA-29D4193B3408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="0" windowWidth="24960" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIMVASTATIN" sheetId="1" r:id="rId1"/>
@@ -2312,7 +2312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2328,10 +2328,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2347,7 +2346,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2646,117 +2645,117 @@
   <dimension ref="A1:CY134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="69.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="69.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" customWidth="1"/>
+    <col min="7" max="7" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.5" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" customWidth="1"/>
     <col min="14" max="14" width="32.6640625" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="26" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="22.6640625" customWidth="1"/>
-    <col min="32" max="32" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="122" customWidth="1"/>
     <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="17" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="10" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="16" bestFit="1" customWidth="1"/>
-    <col min="73" max="74" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="74" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="31" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="24" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="27" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="20" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:103" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>616</v>
       </c>
@@ -2769,7 +2768,7 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" t="s">
         <v>618</v>
       </c>
       <c r="F1" t="s">
@@ -3067,7 +3066,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7661</v>
       </c>
@@ -3300,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7662</v>
       </c>
@@ -3533,7 +3532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3975</v>
       </c>
@@ -3751,7 +3750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3976</v>
       </c>
@@ -3969,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3977</v>
       </c>
@@ -4202,7 +4201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4513</v>
       </c>
@@ -4435,7 +4434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4514</v>
       </c>
@@ -4668,9 +4667,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5547</v>
+        <v>1115547</v>
       </c>
       <c r="B9">
         <v>272210203</v>
@@ -4901,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4370</v>
       </c>
@@ -5134,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4371</v>
       </c>
@@ -5340,7 +5339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4272</v>
       </c>
@@ -5573,7 +5572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7983</v>
       </c>
@@ -5803,7 +5802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7984</v>
       </c>
@@ -6036,7 +6035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8147</v>
       </c>
@@ -6254,7 +6253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3771</v>
       </c>
@@ -6460,7 +6459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3772</v>
       </c>
@@ -6693,7 +6692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3773</v>
       </c>
@@ -6899,7 +6898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3775</v>
       </c>
@@ -7132,7 +7131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3776</v>
       </c>
@@ -7365,7 +7364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3777</v>
       </c>
@@ -7598,7 +7597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3778</v>
       </c>
@@ -7831,7 +7830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>7095</v>
       </c>
@@ -8064,7 +8063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7106</v>
       </c>
@@ -8288,7 +8287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3864</v>
       </c>
@@ -8506,7 +8505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3866</v>
       </c>
@@ -8724,7 +8723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3820</v>
       </c>
@@ -8957,7 +8956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3821</v>
       </c>
@@ -9190,7 +9189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3827</v>
       </c>
@@ -9423,7 +9422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3829</v>
       </c>
@@ -9656,7 +9655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2166</v>
       </c>
@@ -9889,7 +9888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3426</v>
       </c>
@@ -10095,7 +10094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3427</v>
       </c>
@@ -10328,7 +10327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3428</v>
       </c>
@@ -10561,7 +10560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3441</v>
       </c>
@@ -10794,7 +10793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3442</v>
       </c>
@@ -11027,7 +11026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3447</v>
       </c>
@@ -11260,7 +11259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3448</v>
       </c>
@@ -11466,7 +11465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3449</v>
       </c>
@@ -11699,7 +11698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3542</v>
       </c>
@@ -11902,7 +11901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>3543</v>
       </c>
@@ -12135,7 +12134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3544</v>
       </c>
@@ -12368,7 +12367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>3622</v>
       </c>
@@ -12574,7 +12573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>3623</v>
       </c>
@@ -12792,7 +12791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>3624</v>
       </c>
@@ -13025,7 +13024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>3625</v>
       </c>
@@ -13258,7 +13257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>3626</v>
       </c>
@@ -13464,7 +13463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>3627</v>
       </c>
@@ -13700,7 +13699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>3628</v>
       </c>
@@ -13906,7 +13905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>3629</v>
       </c>
@@ -14142,7 +14141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>3632</v>
       </c>
@@ -14375,7 +14374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>3697</v>
       </c>
@@ -14593,7 +14592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>3698</v>
       </c>
@@ -14826,7 +14825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2076</v>
       </c>
@@ -15059,7 +15058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2077</v>
       </c>
@@ -15292,7 +15291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>6790</v>
       </c>
@@ -15522,7 +15521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>6814</v>
       </c>
@@ -15752,7 +15751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>11233</v>
       </c>
@@ -15970,7 +15969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>8267</v>
       </c>
@@ -16203,7 +16202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>8268</v>
       </c>
@@ -16436,7 +16435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>8269</v>
       </c>
@@ -16669,7 +16668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>4572</v>
       </c>
@@ -16902,7 +16901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>4573</v>
       </c>
@@ -17135,7 +17134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>4066</v>
       </c>
@@ -17368,7 +17367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>4067</v>
       </c>
@@ -17604,7 +17603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>4068</v>
       </c>
@@ -17837,7 +17836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>4069</v>
       </c>
@@ -18049,7 +18048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4214</v>
       </c>
@@ -18282,7 +18281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>4215</v>
       </c>
@@ -18515,7 +18514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>4226</v>
       </c>
@@ -18733,7 +18732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>4227</v>
       </c>
@@ -18939,7 +18938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>4207</v>
       </c>
@@ -19172,7 +19171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>4208</v>
       </c>
@@ -19405,7 +19404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>4080</v>
       </c>
@@ -19638,7 +19637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4081</v>
       </c>
@@ -19871,7 +19870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>5160</v>
       </c>
@@ -20104,7 +20103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>5161</v>
       </c>
@@ -20337,7 +20336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>4954</v>
       </c>
@@ -20543,7 +20542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4519</v>
       </c>
@@ -20749,7 +20748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4520</v>
       </c>
@@ -20967,7 +20966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>7520</v>
       </c>
@@ -21197,7 +21196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>5045</v>
       </c>
@@ -21430,7 +21429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>5046</v>
       </c>
@@ -21663,7 +21662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>5052</v>
       </c>
@@ -21881,7 +21880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>5053</v>
       </c>
@@ -22099,7 +22098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>5054</v>
       </c>
@@ -22311,7 +22310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>5055</v>
       </c>
@@ -22529,7 +22528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>5056</v>
       </c>
@@ -22735,7 +22734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4391</v>
       </c>
@@ -22968,7 +22967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>7620</v>
       </c>
@@ -23171,7 +23170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>7621</v>
       </c>
@@ -23374,7 +23373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>5783</v>
       </c>
@@ -23580,7 +23579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>5784</v>
       </c>
@@ -23786,7 +23785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>3405</v>
       </c>
@@ -24019,7 +24018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>3406</v>
       </c>
@@ -24252,7 +24251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>3408</v>
       </c>
@@ -24455,7 +24454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>3409</v>
       </c>
@@ -24688,7 +24687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>4273</v>
       </c>
@@ -24921,7 +24920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4274</v>
       </c>
@@ -25157,7 +25156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>4282</v>
       </c>
@@ -25390,7 +25389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>4283</v>
       </c>
@@ -25623,7 +25622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>4194</v>
       </c>
@@ -25829,7 +25828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>4195</v>
       </c>
@@ -26041,7 +26040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>8351</v>
       </c>
@@ -26271,7 +26270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>4602</v>
       </c>
@@ -26489,7 +26488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>4603</v>
       </c>
@@ -26722,7 +26721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>5196</v>
       </c>
@@ -26955,7 +26954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>4825</v>
       </c>
@@ -27167,7 +27166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1556</v>
       </c>
@@ -27400,7 +27399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1557</v>
       </c>
@@ -27633,7 +27632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>4677</v>
       </c>
@@ -27866,7 +27865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>4109</v>
       </c>
@@ -28099,7 +28098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>4110</v>
       </c>
@@ -28332,7 +28331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>4644</v>
       </c>
@@ -28565,7 +28564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>4645</v>
       </c>
@@ -28786,7 +28785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>4687</v>
       </c>
@@ -29013,7 +29012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>4688</v>
       </c>
@@ -29240,7 +29239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>5216</v>
       </c>
@@ -29443,7 +29442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>5217</v>
       </c>
@@ -29676,7 +29675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>3453</v>
       </c>
@@ -29909,7 +29908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>3454</v>
       </c>
@@ -30142,7 +30141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>1555</v>
       </c>
@@ -30375,7 +30374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>4673</v>
       </c>
@@ -30608,7 +30607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>4674</v>
       </c>
@@ -30841,7 +30840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>4675</v>
       </c>
@@ -31074,7 +31073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>4147</v>
       </c>
@@ -31310,7 +31309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>4161</v>
       </c>
@@ -31543,7 +31542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>4162</v>
       </c>
@@ -31776,7 +31775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>9166</v>
       </c>
@@ -32006,7 +32005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>9164</v>
       </c>
@@ -32236,7 +32235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>9328</v>
       </c>
@@ -32466,7 +32465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>9892</v>
       </c>
@@ -32696,7 +32695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>9893</v>
       </c>
@@ -32926,7 +32925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>9894</v>
       </c>
@@ -33169,114 +33168,114 @@
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="31.33203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="34" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="26" style="2" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="26.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="26.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="26.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="28.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="22.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="19.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="3.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="25.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="26.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="3.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="25.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="24.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="73" max="74" width="23.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="73" max="74" width="23.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="22.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="31" style="2" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="23.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="27.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="21.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="23.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="25.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="4.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="27.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="21.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="23.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="26.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="25.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="4.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="30.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="30.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="21.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="104" max="16384" width="9.1640625" style="2"/>
+    <col min="103" max="103" width="21.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="104" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:103" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>616</v>
       </c>
@@ -33587,7 +33586,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>267</v>
       </c>
@@ -33820,7 +33819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>268</v>
       </c>
@@ -34047,7 +34046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>269</v>
       </c>
@@ -34280,7 +34279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>270</v>
       </c>
@@ -34527,113 +34526,113 @@
       <selection activeCell="AI1" sqref="AI1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="55.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
     <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.1640625" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.109375" customWidth="1"/>
+    <col min="15" max="15" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="26" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="105" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="17" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="10" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="16" bestFit="1" customWidth="1"/>
-    <col min="73" max="74" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="74" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="15.1640625" customWidth="1"/>
-    <col min="78" max="78" width="16.1640625" customWidth="1"/>
+    <col min="77" max="77" width="15.109375" customWidth="1"/>
+    <col min="78" max="78" width="16.109375" customWidth="1"/>
     <col min="79" max="79" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="31" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="24" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="27" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="20" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>616</v>
       </c>
@@ -34944,7 +34943,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7666</v>
       </c>
@@ -35168,7 +35167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>105</v>
       </c>
@@ -35401,7 +35400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>106</v>
       </c>
@@ -35610,7 +35609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>107</v>
       </c>
@@ -35837,7 +35836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3444</v>
       </c>
@@ -36046,7 +36045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2103</v>
       </c>
@@ -36255,7 +36254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2104</v>
       </c>
@@ -36464,7 +36463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2109</v>
       </c>
@@ -36691,7 +36690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2110</v>
       </c>
@@ -36924,7 +36923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2111</v>
       </c>
@@ -37133,7 +37132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2112</v>
       </c>
@@ -37360,7 +37359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2113</v>
       </c>
@@ -37593,7 +37592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6667</v>
       </c>
@@ -37814,7 +37813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>20073</v>
       </c>
@@ -38037,113 +38036,113 @@
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="66.5" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="66.44140625" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
-    <col min="6" max="6" width="65.5" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.5" customWidth="1"/>
+    <col min="6" max="6" width="65.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.44140625" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="35.5" customWidth="1"/>
-    <col min="15" max="15" width="11.5" customWidth="1"/>
-    <col min="16" max="16" width="8.1640625" customWidth="1"/>
-    <col min="17" max="17" width="9.5" customWidth="1"/>
+    <col min="14" max="14" width="35.44140625" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" customWidth="1"/>
+    <col min="16" max="16" width="8.109375" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" customWidth="1"/>
     <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="26" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="181.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="181.44140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="17" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="10" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="16" bestFit="1" customWidth="1"/>
-    <col min="73" max="74" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="74" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="31" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="24" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="27" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="20" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:103" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>616</v>
       </c>
@@ -38454,7 +38453,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5149</v>
       </c>
@@ -38687,7 +38686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5150</v>
       </c>
@@ -38920,7 +38919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4356</v>
       </c>
@@ -39153,7 +39152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4358</v>
       </c>
@@ -39386,7 +39385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2719</v>
       </c>
@@ -39613,7 +39612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2720</v>
       </c>
@@ -39840,7 +39839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4515</v>
       </c>
@@ -40046,7 +40045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4516</v>
       </c>
@@ -40252,7 +40251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4303</v>
       </c>
@@ -40470,7 +40469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4304</v>
       </c>
@@ -40688,7 +40687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6236</v>
       </c>
@@ -40921,7 +40920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6237</v>
       </c>
@@ -41154,7 +41153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4305</v>
       </c>
@@ -41372,7 +41371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4306</v>
       </c>
@@ -41590,7 +41589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4307</v>
       </c>
@@ -41823,7 +41822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4308</v>
       </c>
@@ -42029,7 +42028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4309</v>
       </c>
@@ -42262,7 +42261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4319</v>
       </c>
@@ -42498,7 +42497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4320</v>
       </c>
@@ -42734,7 +42733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>6179</v>
       </c>
@@ -42967,7 +42966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>6180</v>
       </c>
@@ -43200,7 +43199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4269</v>
       </c>
@@ -43406,7 +43405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4270</v>
       </c>
@@ -43642,7 +43641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>7812</v>
       </c>
@@ -43875,7 +43874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:101" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>7813</v>
       </c>
@@ -44108,7 +44107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8145</v>
       </c>
@@ -44338,7 +44337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>8144</v>
       </c>
@@ -44568,7 +44567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1912</v>
       </c>
@@ -44801,7 +44800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1913</v>
       </c>
@@ -45034,7 +45033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>5842</v>
       </c>
@@ -45252,7 +45251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>5843</v>
       </c>
@@ -45470,7 +45469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4574</v>
       </c>
@@ -45673,7 +45672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4575</v>
       </c>
@@ -45891,7 +45890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4576</v>
       </c>
@@ -46106,7 +46105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4577</v>
       </c>
@@ -46324,7 +46323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4749</v>
       </c>
@@ -46542,7 +46541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4229</v>
       </c>
@@ -46775,7 +46774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4230</v>
       </c>
@@ -47008,7 +47007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4233</v>
       </c>
@@ -47214,7 +47213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>5392</v>
       </c>
@@ -47420,7 +47419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>5393</v>
       </c>
@@ -47653,7 +47652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>5394</v>
       </c>
@@ -47874,7 +47873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5397</v>
       </c>
@@ -48101,7 +48100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>5398</v>
       </c>
@@ -48328,7 +48327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>5047</v>
       </c>
@@ -48564,7 +48563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>5048</v>
       </c>
@@ -48797,7 +48796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>5049</v>
       </c>
@@ -49033,7 +49032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4462</v>
       </c>
@@ -49245,7 +49244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>4463</v>
       </c>
@@ -49463,7 +49462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4464</v>
       </c>
@@ -49675,7 +49674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>4465</v>
       </c>
@@ -49887,7 +49886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>4470</v>
       </c>
@@ -50105,7 +50104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>4471</v>
       </c>
@@ -50338,7 +50337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>4472</v>
       </c>
@@ -50556,7 +50555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>4473</v>
       </c>
@@ -50789,7 +50788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>4476</v>
       </c>
@@ -51022,7 +51021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>4477</v>
       </c>
@@ -51255,7 +51254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>4750</v>
       </c>
@@ -51488,7 +51487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>4751</v>
       </c>
@@ -51694,7 +51693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>4752</v>
       </c>
@@ -51927,7 +51926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>7732</v>
       </c>
@@ -52163,7 +52162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>7755</v>
       </c>
@@ -52396,7 +52395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>4715</v>
       </c>
@@ -52614,7 +52613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>4716</v>
       </c>
@@ -52847,7 +52846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>5433</v>
       </c>
@@ -53080,7 +53079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>5434</v>
       </c>
@@ -53313,7 +53312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>5478</v>
       </c>
@@ -53519,7 +53518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>5479</v>
       </c>
@@ -53725,7 +53724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>4618</v>
       </c>
@@ -53943,7 +53942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>4619</v>
       </c>
@@ -54170,7 +54169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>8816</v>
       </c>
@@ -54388,7 +54387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>8817</v>
       </c>
@@ -54606,7 +54605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>4823</v>
       </c>
@@ -54839,7 +54838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4824</v>
       </c>
@@ -55072,7 +55071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>4689</v>
       </c>
@@ -55305,7 +55304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>4690</v>
       </c>
@@ -55526,7 +55525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>4691</v>
       </c>
@@ -55762,7 +55761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4635</v>
       </c>
@@ -55995,7 +55994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4636</v>
       </c>
@@ -56228,7 +56227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>5976</v>
       </c>
@@ -56464,7 +56463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>5467</v>
       </c>
@@ -56697,7 +56696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>5468</v>
       </c>
@@ -56930,7 +56929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4154</v>
       </c>
@@ -57163,7 +57162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4155</v>
       </c>
@@ -57396,7 +57395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4156</v>
       </c>
@@ -57632,7 +57631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4157</v>
       </c>
@@ -57868,7 +57867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>9062</v>
       </c>
@@ -58086,7 +58085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>9063</v>
       </c>

</xml_diff>